<commit_message>
commit to check CICD
</commit_message>
<xml_diff>
--- a/src/main/java/nandha/resources/testdata.xlsx
+++ b/src/main/java/nandha/resources/testdata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>searchdata</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>₹33,999</t>
+  </si>
+  <si>
+    <t>18 Aug, Sunday</t>
+  </si>
+  <si>
+    <t>₹15,194</t>
   </si>
 </sst>
 </file>
@@ -640,13 +646,13 @@
         <v>636903</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>